<commit_message>
feature jumlah nama & Kategori Warna, Text size calculation
</commit_message>
<xml_diff>
--- a/test-nama.xlsx
+++ b/test-nama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Documents\a_Kelvin_a\Code\Phyton\Freelance\alpha_digital\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEE4F20-326A-451C-B352-7A3E84705CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043B8CC0-1C8C-4F2A-BBC4-D9CEA3476962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{61AEB1A2-1B83-4C6C-91F3-2D4FF69640B5}"/>
   </bookViews>
@@ -25,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Alice</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
   <si>
     <t>Carol</t>
   </si>
@@ -48,12 +36,6 @@
     <t>Eve</t>
   </si>
   <si>
-    <t>Frank</t>
-  </si>
-  <si>
-    <t>Grace</t>
-  </si>
-  <si>
     <t>Henry</t>
   </si>
   <si>
@@ -69,13 +51,151 @@
     <t>Liam</t>
   </si>
   <si>
-    <t>Mia</t>
-  </si>
-  <si>
-    <t>Noah</t>
-  </si>
-  <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Haikal Muqowwi</t>
+  </si>
+  <si>
+    <t>Azri Ardha</t>
+  </si>
+  <si>
+    <t>Akifa Ayanna</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ALFIN MASHLUKHI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ARYA BALANGGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DANISA FAHMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IMELDA PUTRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KAMILA INA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KHOIRUL ABIDILLAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KHOIRUN NISA'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HARUN ARROSYID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MAGHFIROTUL FITRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FALICHUDIN ZUHRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DENI KHURNIAWAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MUTOHHARUL JANAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> REZA PUTRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MUHAMMAD ROFIUDIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NAJWA FAIQOTUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NIHAYYATUZZAIM MA'LA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RIVANO AHMAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ZAZQIA AYU</t>
+  </si>
+  <si>
+    <t> AZILDAN MAULANA</t>
+  </si>
+  <si>
+    <t>NURI</t>
+  </si>
+  <si>
+    <t>PUSPARENI</t>
+  </si>
+  <si>
+    <t>ENDAH</t>
+  </si>
+  <si>
+    <t>YUMNA</t>
+  </si>
+  <si>
+    <t>EMA</t>
+  </si>
+  <si>
+    <t>RIVANKA</t>
+  </si>
+  <si>
+    <t>RIKA</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>ANIS</t>
+  </si>
+  <si>
+    <t>URIE</t>
+  </si>
+  <si>
+    <t>KARIN</t>
+  </si>
+  <si>
+    <t>IRA</t>
+  </si>
+  <si>
+    <t>FEBI</t>
+  </si>
+  <si>
+    <t>RANI</t>
+  </si>
+  <si>
+    <t>ZAFRA</t>
+  </si>
+  <si>
+    <t>INDRA</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Hijau</t>
+  </si>
+  <si>
+    <t>Biru</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>Universitas Tarumanegara</t>
+  </si>
+  <si>
+    <t>UNIVERSITAS TARUMANEGARA</t>
+  </si>
+  <si>
+    <t>Franky</t>
+  </si>
+  <si>
+    <t>Gracious</t>
+  </si>
+  <si>
+    <t>Tosca</t>
   </si>
 </sst>
 </file>
@@ -436,98 +556,451 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8ED79CB-37F0-4FB2-AC61-2EAFA9904B10}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>1</v>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>